<commit_message>
actualización y eliminación de IIEE y personal
</commit_message>
<xml_diff>
--- a/src/archives/reporte.xlsx
+++ b/src/archives/reporte.xlsx
@@ -53,85 +53,52 @@
     <t xml:space="preserve">OBSERVACIONES</t>
   </si>
   <si>
-    <t xml:space="preserve">12345678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">juan lopez paiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-07-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07:55:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:04:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56 minutos</t>
+    <t xml:space="preserve">87548754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yanet altamirano quiroz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:50:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:05:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:03:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:44:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:53:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:53:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:53:39</t>
   </si>
   <si>
     <t xml:space="preserve">Tiene horas sin marcar</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08:50:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:55:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14:17:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16:44:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1h 12 minutos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-07-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07:55:53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:03:49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14:11:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17:36:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 minutos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-07-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07:53:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-07-07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07:50:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:31:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-07-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08:52:27</t>
+    <t xml:space="preserve">2025-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:52:27</t>
   </si>
   <si>
     <t xml:space="preserve">14:14:52</t>
@@ -140,10 +107,7 @@
     <t xml:space="preserve">18:10:06</t>
   </si>
   <si>
-    <t xml:space="preserve">52 minutos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-07-11</t>
+    <t xml:space="preserve">2025-03-16</t>
   </si>
   <si>
     <t xml:space="preserve">07:51:52</t>
@@ -156,6 +120,12 @@
   </si>
   <si>
     <t xml:space="preserve">17:53:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12345667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carla siares adrianzen</t>
   </si>
 </sst>
 </file>
@@ -525,13 +495,17 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="F2"/>
-      <c r="G2"/>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -542,22 +516,20 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
       </c>
       <c r="I3" t="s">
         <v>22</v>
@@ -576,17 +548,15 @@
       <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4"/>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
@@ -600,100 +570,133 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6"/>
-      <c r="G6"/>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregar turnos y horarios de trabajo a IIEE, turnos para los trabajadores
</commit_message>
<xml_diff>
--- a/src/archives/reporte.xlsx
+++ b/src/archives/reporte.xlsx
@@ -53,13 +53,76 @@
     <t xml:space="preserve">OBSERVACIONES</t>
   </si>
   <si>
-    <t xml:space="preserve">87548754</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yanet altamirano quiroz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-03-13</t>
+    <t xml:space="preserve">12345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juan lopez paiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-07-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:55:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:04:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiene horas sin marcar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87654321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juan garcia flores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-07-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:52:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:55:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:46:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-07-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:59:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-07-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08:50:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:55:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:17:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:44:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h 12 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve">07:55:53</t>
@@ -74,61 +137,43 @@
     <t xml:space="preserve">17:36:28</t>
   </si>
   <si>
-    <t xml:space="preserve">0 minutos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-03-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07:50:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:05:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14:03:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18:44:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12345667</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carla siares adrianzen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-03-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07:55:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:04:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiene horas sin marcar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-03-18</t>
+    <t xml:space="preserve">2023-07-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:56:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:03:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:17:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:21:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-06-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-07-13</t>
   </si>
   <si>
     <t xml:space="preserve">07:53:38</t>
   </si>
   <si>
-    <t xml:space="preserve">13:53:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17:53:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-03-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07:52:27</t>
+    <t xml:space="preserve">07:50:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:31:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-07-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08:52:27</t>
   </si>
   <si>
     <t xml:space="preserve">14:14:52</t>
@@ -137,7 +182,28 @@
     <t xml:space="preserve">18:10:06</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-03-16</t>
+    <t xml:space="preserve">52 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:58:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:58:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:39:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-07-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:41:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:58:58</t>
   </si>
   <si>
     <t xml:space="preserve">07:51:52</t>
@@ -152,19 +218,58 @@
     <t xml:space="preserve">17:53:26</t>
   </si>
   <si>
-    <t xml:space="preserve">16:36:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 minutos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-03-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07:50:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:31:46</t>
+    <t xml:space="preserve">07:44:32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:00:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:00:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:26:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:05:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:15:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:55:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54871287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carla palacios gomez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:20:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:13:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:12:22</t>
   </si>
 </sst>
 </file>
@@ -534,25 +639,21 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -563,42 +664,38 @@
       <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3"/>
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
+      <c r="E4"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -609,23 +706,25 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="F5"/>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6">
@@ -636,12 +735,14 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="E6"/>
       <c r="F6" t="s">
         <v>35</v>
       </c>
@@ -649,18 +750,18 @@
         <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -678,39 +779,31 @@
         <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>41</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -721,179 +814,434 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I9" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
       <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10"/>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" t="s">
-        <v>36</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I10" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F12"/>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="H12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13"/>
       <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" t="s">
-        <v>42</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G13"/>
       <c r="H13" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="I13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
         <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" t="s">
-        <v>46</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I14" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15"/>
-      <c r="G15"/>
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" t="s">
+        <v>63</v>
+      </c>
       <c r="H15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="I15" t="s">
-        <v>28</v>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>